<commit_message>
Modifies epidemic model outputs and r_U parameter values to allow better test and trace simulations. Adds visualization.py to hold plotting templates (first implemented).
</commit_message>
<xml_diff>
--- a/documentation/transition_matrix_w_sens_spec_simplified.xlsx
+++ b/documentation/transition_matrix_w_sens_spec_simplified.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ljneuvon/Work/Epidemic control/Covid_policies_w_imperfect_testing/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28A6E86-3679-9B4E-8128-9619ABFBD062}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112F9655-EB57-744A-9C1E-D6D0461034CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39060" yWindow="4260" windowWidth="28800" windowHeight="12280" xr2:uid="{59EEBB9C-DF2A-EC4F-BD0B-CDAFEE3749BE}"/>
+    <workbookView xWindow="39040" yWindow="4240" windowWidth="28800" windowHeight="12280" xr2:uid="{59EEBB9C-DF2A-EC4F-BD0B-CDAFEE3749BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -559,13 +559,15 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="13.1640625" customWidth="1"/>
     <col min="6" max="6" width="12.1640625" customWidth="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>